<commit_message>
Add transaction format string to excel currencies table
</commit_message>
<xml_diff>
--- a/Private Markets Portfolio.xlsx
+++ b/Private Markets Portfolio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hextpoint-my.sharepoint.com/personal/lawrence_dwight_hextpoint_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LawrenceDwight\repos\Private Markets Portfolio Report\PrivateMarketsPortfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1299" documentId="8_{1B316B56-986E-49D6-8624-A48DFF96A703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{963D4FBE-D023-4C9B-A0DC-AD376A5E1CB9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFB2BA2-F746-404E-A510-EDCCA7E651A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="380" yWindow="380" windowWidth="28800" windowHeight="15370" xr2:uid="{9E72535B-9A24-451E-AA73-D07C6100DA90}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15370" xr2:uid="{9E72535B-9A24-451E-AA73-D07C6100DA90}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="18" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4441" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4445" uniqueCount="175">
   <si>
     <t>WebURL</t>
   </si>
@@ -562,6 +562,18 @@
   <si>
     <t>Co-Investment</t>
   </si>
+  <si>
+    <t>Transaction format string</t>
+  </si>
+  <si>
+    <t>\€#,0.00;(\€#,0.00);\€#,0.00</t>
+  </si>
+  <si>
+    <t>\$#,0.00;(\$#,0.00);\$#,0.00</t>
+  </si>
+  <si>
+    <t>\£#,0.00;(\£#,0.00);\£#,0.00</t>
+  </si>
 </sst>
 </file>
 
@@ -655,10 +667,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{CB4E5208-4831-42B1-9EB1-C8F489C532FB}" name="Settings" displayName="Settings" ref="A1:B2" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{CB4E5208-4831-42B1-9EB1-C8F489C532FB}"/>
@@ -713,13 +721,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31AFFF4A-63E6-47CF-9870-54CF7C46E767}" name="Currencies" displayName="Currencies" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4" xr:uid="{31AFFF4A-63E6-47CF-9870-54CF7C46E767}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31AFFF4A-63E6-47CF-9870-54CF7C46E767}" name="Currencies" displayName="Currencies" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4" xr:uid="{31AFFF4A-63E6-47CF-9870-54CF7C46E767}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3DDE46DD-804F-44C8-AEEE-7FEE02D8B3E7}" name="Currency Name"/>
     <tableColumn id="2" xr3:uid="{52F7E188-7594-4F96-B007-B181D5828C1B}" name="CCY"/>
     <tableColumn id="3" xr3:uid="{4E09777C-FE4D-40AF-B292-619561EF68D9}" name="Currency Symbol"/>
     <tableColumn id="4" xr3:uid="{0FF52081-5739-44E9-97C9-5D5793E3C062}" name="Currency format string"/>
+    <tableColumn id="6" xr3:uid="{7947D1B0-5AFD-4068-A6DA-74F0C0C23464}" name="Transaction format string"/>
     <tableColumn id="5" xr3:uid="{F6EA3956-2A73-4DA8-A497-9E2B7F2551B1}" name="Reporting Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -27297,20 +27306,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88B6FA8-A118-496C-A90C-3675EE10BAC5}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.7265625" customWidth="1"/>
     <col min="3" max="3" width="17.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
+    <col min="4" max="5" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -27324,10 +27333,13 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -27340,14 +27352,17 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="b">
+      <c r="E2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -27360,11 +27375,14 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="b">
+      <c r="E3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -27377,13 +27395,16 @@
       <c r="D4" t="s">
         <v>164</v>
       </c>
-      <c r="E4" t="b">
+      <c r="E4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{750912B2-39A5-4969-935A-06DBD3D6C461}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{750912B2-39A5-4969-935A-06DBD3D6C461}">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>